<commit_message>
Worked on the Refactor action
git-svn-id: http://tps.ics.uci.edu/svn/projects/simse/trunk/simse@5226 3eb8784e-3aee-0310-b028-d3d3d21a5a25
</commit_message>
<xml_diff>
--- a/res/models/xp/TestData.xlsx
+++ b/res/models/xp/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>CreateUserStories</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Program (J, R, P, S)</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Everything wrong</t>
   </si>
 </sst>
 </file>
@@ -455,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,6 +718,30 @@
       </c>
       <c r="C27">
         <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added & tested rule attached to the refactor action that causes errors to be introduced into the code.
git-svn-id: http://tps.ics.uci.edu/svn/projects/simse/trunk/simse@5325 3eb8784e-3aee-0310-b028-d3d3d21a5a25
</commit_message>
<xml_diff>
--- a/res/models/xp/TestData.xlsx
+++ b/res/models/xp/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>CreateUserStories</t>
   </si>
@@ -126,10 +126,31 @@
     <t>Program (J, R, P, S)</t>
   </si>
   <si>
-    <t>Refactoring</t>
-  </si>
-  <si>
     <t>Everything wrong</t>
+  </si>
+  <si>
+    <t>Refactoring - duration</t>
+  </si>
+  <si>
+    <t>Refactoring - num errors introduced</t>
+  </si>
+  <si>
+    <t>6 errors, no coding standard, no refactoring tool (everything wrong)</t>
+  </si>
+  <si>
+    <t>0 errors, no coding standard, no refactoring tool</t>
+  </si>
+  <si>
+    <t>6 errors, no refactoring tool</t>
+  </si>
+  <si>
+    <t>6 errors, no coding standard</t>
+  </si>
+  <si>
+    <t>0 errors, no refactoring tool</t>
+  </si>
+  <si>
+    <t>0 errors, no coding standard</t>
   </si>
 </sst>
 </file>
@@ -461,15 +482,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -722,7 +743,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
@@ -738,10 +759,71 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued working on integrate actions and rules.
git-svn-id: http://tps.ics.uci.edu/svn/projects/simse/trunk/simse@5328 3eb8784e-3aee-0310-b028-d3d3d21a5a25
</commit_message>
<xml_diff>
--- a/res/models/xp/TestData.xlsx
+++ b/res/models/xp/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>CreateUserStories</t>
   </si>
@@ -151,6 +151,54 @@
   </si>
   <si>
     <t>0 errors, no coding standard</t>
+  </si>
+  <si>
+    <t>Pair-integration</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Errors introduced into code</t>
+  </si>
+  <si>
+    <t>Only one pair - everything right</t>
+  </si>
+  <si>
+    <t>Two pairs - everything right</t>
+  </si>
+  <si>
+    <t>All pairs - everything right</t>
+  </si>
+  <si>
+    <t>No coding standard</t>
+  </si>
+  <si>
+    <t>0% refactored</t>
+  </si>
+  <si>
+    <t>50% refactored</t>
+  </si>
+  <si>
+    <t>100% erroneous code</t>
+  </si>
+  <si>
+    <t>12% erroneous code</t>
+  </si>
+  <si>
+    <t>No coding standard, 0% refactored, 100% erroneous code (everything wrong)</t>
+  </si>
+  <si>
+    <t>0% refactored, 0% erroneous code</t>
+  </si>
+  <si>
+    <t>0% refactored, no coding standard, 0% erroneous code</t>
+  </si>
+  <si>
+    <t>100% refactored, 6% erroneous code</t>
+  </si>
+  <si>
+    <t>50% refactored, 3% erroneous code</t>
   </si>
 </sst>
 </file>
@@ -482,15 +530,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="62" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -765,12 +813,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -778,7 +826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -786,7 +834,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -794,7 +842,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -802,7 +850,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -810,7 +858,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -818,12 +866,100 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>44</v>
       </c>
       <c r="B40">
         <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43">
+        <v>43</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45">
+        <v>17</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fine tuning of the pair-integrate actions
git-svn-id: http://tps.ics.uci.edu/svn/projects/simse/trunk/simse@5373 3eb8784e-3aee-0310-b028-d3d3d21a5a25
</commit_message>
<xml_diff>
--- a/res/models/xp/TestData.xlsx
+++ b/res/models/xp/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>CreateUserStories</t>
   </si>
@@ -183,22 +183,25 @@
     <t>100% erroneous code</t>
   </si>
   <si>
-    <t>12% erroneous code</t>
-  </si>
-  <si>
-    <t>No coding standard, 0% refactored, 100% erroneous code (everything wrong)</t>
-  </si>
-  <si>
-    <t>0% refactored, 0% erroneous code</t>
-  </si>
-  <si>
     <t>0% refactored, no coding standard, 0% erroneous code</t>
   </si>
   <si>
     <t>100% refactored, 6% erroneous code</t>
   </si>
   <si>
-    <t>50% refactored, 3% erroneous code</t>
+    <t>&gt; 12</t>
+  </si>
+  <si>
+    <t>No coding standard, 0% refactored, 86% erroneous code (everything wrong)</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>10% erroneous code</t>
+  </si>
+  <si>
+    <t>53% refactored, 3% erroneous code</t>
   </si>
 </sst>
 </file>
@@ -234,8 +237,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -900,6 +906,12 @@
       <c r="A44" t="s">
         <v>49</v>
       </c>
+      <c r="B44">
+        <v>24</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
@@ -914,52 +926,101 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="B46">
+        <v>34</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>51</v>
       </c>
+      <c r="B47">
+        <v>21</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48">
+        <v>21</v>
+      </c>
+      <c r="C48">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49">
+        <v>29</v>
+      </c>
+      <c r="C49">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50">
+        <v>26</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51">
+        <v>18</v>
+      </c>
+      <c r="C51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52">
+        <v>38</v>
+      </c>
+      <c r="C52">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
+        <v>56</v>
+      </c>
+      <c r="B53">
+        <v>18</v>
+      </c>
+      <c r="C53">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="B54">
+        <v>19</v>
+      </c>
+      <c r="C54">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and tested integrate action
git-svn-id: http://tps.ics.uci.edu/svn/projects/simse/trunk/simse@5433 3eb8784e-3aee-0310-b028-d3d3d21a5a25
</commit_message>
<xml_diff>
--- a/res/models/xp/TestData.xlsx
+++ b/res/models/xp/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>CreateUserStories</t>
   </si>
@@ -202,6 +202,27 @@
   </si>
   <si>
     <t>53% refactored, 3% erroneous code</t>
+  </si>
+  <si>
+    <t>100% design, 100% unit tests</t>
+  </si>
+  <si>
+    <t>122 ticks</t>
+  </si>
+  <si>
+    <t>134 ticks</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>All emps - everything right</t>
+  </si>
+  <si>
+    <t>4 emps - everything right</t>
+  </si>
+  <si>
+    <t>2 emps - everything right</t>
   </si>
 </sst>
 </file>
@@ -536,491 +557,608 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="70.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>49</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>61</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>54</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>32</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>61</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>41</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>122</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="F3" t="s">
+    <row r="3" spans="1:9">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="F4" t="s">
+    <row r="4" spans="1:9">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10">
         <v>57</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>100</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>35</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>46</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>32</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>33</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>34</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>28</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>52</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>36</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>36</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>32</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>36</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>69</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>61</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>37</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>24</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>36</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>24</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>39</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>40</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>41</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>42</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>43</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>44</v>
       </c>
-      <c r="B40">
+      <c r="C40">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>45</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>46</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>48</v>
       </c>
-      <c r="B43">
+      <c r="C43">
         <v>43</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>49</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>24</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>50</v>
       </c>
-      <c r="B45">
+      <c r="C45">
         <v>17</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>58</v>
       </c>
-      <c r="B46">
+      <c r="C46">
         <v>34</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>51</v>
       </c>
-      <c r="B47">
+      <c r="C47">
         <v>21</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>52</v>
       </c>
-      <c r="B48">
+      <c r="C48">
         <v>21</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>53</v>
       </c>
-      <c r="B49">
+      <c r="C49">
         <v>29</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>54</v>
       </c>
-      <c r="B50">
+      <c r="C50">
         <v>26</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>60</v>
       </c>
-      <c r="B51">
+      <c r="C51">
         <v>18</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>55</v>
       </c>
-      <c r="B52">
+      <c r="C52">
         <v>38</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>56</v>
       </c>
-      <c r="B53">
+      <c r="C53">
         <v>18</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>61</v>
       </c>
-      <c r="B54">
+      <c r="C54">
         <v>19</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57">
+        <v>47</v>
+      </c>
+      <c r="D57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59">
+        <v>16</v>
+      </c>
+      <c r="D59">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60">
+        <v>31</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62">
+        <v>19</v>
+      </c>
+      <c r="D62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>54</v>
+      </c>
+      <c r="C64">
+        <v>19</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>55</v>
+      </c>
+      <c r="C66">
+        <v>24</v>
+      </c>
+      <c r="D66">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added acceptance testing action.
git-svn-id: http://tps.ics.uci.edu/svn/projects/simse/trunk/simse@5440 3eb8784e-3aee-0310-b028-d3d3d21a5a25
</commit_message>
<xml_diff>
--- a/res/models/xp/TestData.xlsx
+++ b/res/models/xp/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>CreateUserStories</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t>2 emps - everything right</t>
+  </si>
+  <si>
+    <t>Acceptance testing duration: 18 ticks</t>
+  </si>
+  <si>
+    <t>Num tests failed</t>
+  </si>
+  <si>
+    <t>29% erroneous code</t>
   </si>
 </sst>
 </file>
@@ -557,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1159,6 +1168,32 @@
     <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="B70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued testing of scoring
git-svn-id: http://tps.ics.uci.edu/svn/projects/simse/trunk/simse@5594 3eb8784e-3aee-0310-b028-d3d3d21a5a25
</commit_message>
<xml_diff>
--- a/res/models/xp/TestData.xlsx
+++ b/res/models/xp/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="90">
   <si>
     <t>CreateUserStories</t>
   </si>
@@ -270,9 +270,6 @@
     <t>Not using any tools</t>
   </si>
   <si>
-    <t>Not involving the customer in acceptance test creation</t>
-  </si>
-  <si>
     <t>Not using coding standard</t>
   </si>
   <si>
@@ -280,6 +277,15 @@
   </si>
   <si>
     <t>95 if choose to integrate when time's running out, 75 otherwise</t>
+  </si>
+  <si>
+    <t>Doing several development activities at once</t>
+  </si>
+  <si>
+    <t>Saving unit testing 'til the end of each iteration's development</t>
+  </si>
+  <si>
+    <t>63 (integrating when time's running out)</t>
   </si>
 </sst>
 </file>
@@ -614,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1310,30 +1316,44 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
+      <c r="B85">
+        <v>50</v>
+      </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
+      <c r="B86">
+        <v>75</v>
+      </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>86</v>
-      </c>
-      <c r="B88">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added starting narrative, hid attributes, more testing. Version 1.0 of the XP model is now complete.
git-svn-id: http://tps.ics.uci.edu/svn/projects/simse/trunk/simse@5595 3eb8784e-3aee-0310-b028-d3d3d21a5a25
</commit_message>
<xml_diff>
--- a/res/models/xp/TestData.xlsx
+++ b/res/models/xp/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="91">
   <si>
     <t>CreateUserStories</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>63 (integrating when time's running out)</t>
+  </si>
+  <si>
+    <t>90 (integrating when time's running out)</t>
   </si>
 </sst>
 </file>
@@ -623,7 +626,7 @@
   <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1354,6 +1357,9 @@
     <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>